<commit_message>
corrigidas as rotas que haviam sido exclidas anteriormente de delet e edit de estudos, feito melhoria na exclusao que travava a tela
</commit_message>
<xml_diff>
--- a/app/static/uploads/receipts/Modelo25_517760010_2025.xlsx
+++ b/app/static/uploads/receipts/Modelo25_517760010_2025.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>309889669</t>
+          <t>309 889 669</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -451,6 +451,21 @@
       </c>
       <c r="C2" t="n">
         <v>120</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>313424640</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>